<commit_message>
Graphs and text tidied
</commit_message>
<xml_diff>
--- a/ShinyApps/ConditionalSurvival/data/ConditionalSurvival.xlsx
+++ b/ShinyApps/ConditionalSurvival/data/ConditionalSurvival.xlsx
@@ -374,10 +374,10 @@
     <t>curve</t>
   </si>
   <si>
-    <t>Proportion surviving</t>
-  </si>
-  <si>
-    <t>Survival time (years)</t>
+    <t>Life expectancy (years)</t>
+  </si>
+  <si>
+    <t>Survival rate</t>
   </si>
 </sst>
 </file>
@@ -838,9 +838,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,10 +955,10 @@
         <v>97</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>62</v>
@@ -1017,10 +1017,10 @@
         <v>69</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>48</v>
@@ -1079,10 +1079,10 @@
         <v>47</v>
       </c>
       <c r="I4" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>48</v>
@@ -1327,7 +1327,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>